<commit_message>
Updated on 04-20-2024 at 20:33
</commit_message>
<xml_diff>
--- a/experiment_2/data/it.xlsx
+++ b/experiment_2/data/it.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/GitHub/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F740B2-0CAB-3F45-AEDB-E41C08874A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF48F80-F459-C54B-A414-20331037AA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4474,7 +4474,7 @@
   <dimension ref="A1:Q1393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A213" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L233" sqref="L233"/>
+      <selection activeCell="E233" sqref="E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15300,7 +15300,7 @@
       <c r="C218" s="2" t="s">
         <v>1411</v>
       </c>
-      <c r="D218" s="2" t="s">
+      <c r="D218" s="3" t="s">
         <v>233</v>
       </c>
       <c r="E218" s="2">
@@ -15353,7 +15353,7 @@
       <c r="C219" t="s">
         <v>1411</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="3" t="s">
         <v>234</v>
       </c>
       <c r="E219">
@@ -15406,7 +15406,7 @@
       <c r="C220" t="s">
         <v>1411</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="3" t="s">
         <v>235</v>
       </c>
       <c r="E220">
@@ -15459,7 +15459,7 @@
       <c r="C221" t="s">
         <v>1411</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="3" t="s">
         <v>236</v>
       </c>
       <c r="E221">
@@ -15512,7 +15512,7 @@
       <c r="C222" t="s">
         <v>1411</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="3" t="s">
         <v>237</v>
       </c>
       <c r="E222">
@@ -15565,7 +15565,7 @@
       <c r="C223" t="s">
         <v>1411</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="3" t="s">
         <v>238</v>
       </c>
       <c r="E223">
@@ -15618,7 +15618,7 @@
       <c r="C224" t="s">
         <v>1411</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="3" t="s">
         <v>239</v>
       </c>
       <c r="E224">
@@ -15671,7 +15671,7 @@
       <c r="C225" t="s">
         <v>1411</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="3" t="s">
         <v>240</v>
       </c>
       <c r="E225">
@@ -15724,7 +15724,7 @@
       <c r="C226" t="s">
         <v>1411</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="3" t="s">
         <v>241</v>
       </c>
       <c r="E226">
@@ -15777,7 +15777,7 @@
       <c r="C227" t="s">
         <v>1411</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="3" t="s">
         <v>242</v>
       </c>
       <c r="E227">
@@ -15830,7 +15830,7 @@
       <c r="C228" t="s">
         <v>1411</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="3" t="s">
         <v>243</v>
       </c>
       <c r="E228">
@@ -15883,7 +15883,7 @@
       <c r="C229" t="s">
         <v>1411</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="3" t="s">
         <v>244</v>
       </c>
       <c r="E229">
@@ -15936,7 +15936,7 @@
       <c r="C230" t="s">
         <v>1411</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="3" t="s">
         <v>245</v>
       </c>
       <c r="E230">
@@ -15989,7 +15989,7 @@
       <c r="C231" t="s">
         <v>1411</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="3" t="s">
         <v>246</v>
       </c>
       <c r="E231">
@@ -16042,7 +16042,7 @@
       <c r="C232" t="s">
         <v>1411</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="3" t="s">
         <v>247</v>
       </c>
       <c r="E232">
@@ -16095,7 +16095,7 @@
       <c r="C233" t="s">
         <v>1411</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="3" t="s">
         <v>248</v>
       </c>
       <c r="E233">
@@ -16148,7 +16148,7 @@
       <c r="C234" t="s">
         <v>1411</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="3" t="s">
         <v>249</v>
       </c>
       <c r="E234">
@@ -16201,7 +16201,7 @@
       <c r="C235" t="s">
         <v>1411</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="3" t="s">
         <v>250</v>
       </c>
       <c r="E235">
@@ -16254,7 +16254,7 @@
       <c r="C236" t="s">
         <v>1411</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="3" t="s">
         <v>251</v>
       </c>
       <c r="E236">
@@ -16307,7 +16307,7 @@
       <c r="C237" t="s">
         <v>1411</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="3" t="s">
         <v>252</v>
       </c>
       <c r="E237">
@@ -16360,7 +16360,7 @@
       <c r="C238" t="s">
         <v>1411</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="3" t="s">
         <v>253</v>
       </c>
       <c r="E238">
@@ -16413,7 +16413,7 @@
       <c r="C239" t="s">
         <v>1411</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="3" t="s">
         <v>254</v>
       </c>
       <c r="E239">
@@ -16466,7 +16466,7 @@
       <c r="C240" t="s">
         <v>1411</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E240">
@@ -16519,7 +16519,7 @@
       <c r="C241" t="s">
         <v>1411</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="3" t="s">
         <v>256</v>
       </c>
       <c r="E241">
@@ -16572,7 +16572,7 @@
       <c r="C242" t="s">
         <v>1411</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="3" t="s">
         <v>257</v>
       </c>
       <c r="E242">
@@ -16625,7 +16625,7 @@
       <c r="C243" t="s">
         <v>1411</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="3" t="s">
         <v>258</v>
       </c>
       <c r="E243">
@@ -16678,7 +16678,7 @@
       <c r="C244" t="s">
         <v>1411</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="3" t="s">
         <v>259</v>
       </c>
       <c r="E244">

</xml_diff>